<commit_message>
Continuing to improve data provenance
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/data/Curcio_1990_JCompNeurol_HumanPhotoreceptorTopography/DENSITY8_cones_resorted_computedAverage.xlsx
+++ b/data/Curcio_1990_JCompNeurol_HumanPhotoreceptorTopography/DENSITY8_cones_resorted_computedAverage.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="1780" windowWidth="44700" windowHeight="22400" tabRatio="500"/>
+    <workbookView xWindow="1420" yWindow="440" windowWidth="30160" windowHeight="20360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DENSITY8_cones_resorted" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="58">
   <si>
     <t>ALL</t>
   </si>
@@ -71,9 +71,6 @@
     <t>E8746R</t>
   </si>
   <si>
-    <t>average</t>
-  </si>
-  <si>
     <t>counts/mm2</t>
   </si>
   <si>
@@ -198,6 +195,12 @@
   </si>
   <si>
     <t>Pos_36</t>
+  </si>
+  <si>
+    <t>computedAverage</t>
+  </si>
+  <si>
+    <t>reportedAverage</t>
   </si>
 </sst>
 </file>
@@ -512,142 +515,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM38"/>
+  <dimension ref="A1:AM42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="T10" workbookViewId="0">
+      <selection activeCell="AG47" sqref="AG47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>28</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>30</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>31</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>34</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>35</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>36</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>37</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>38</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>39</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>40</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>41</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>44</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>48</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>49</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>50</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>51</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>52</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>53</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>54</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>55</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -766,7 +769,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>166321</v>
@@ -885,7 +888,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4">
         <v>166321</v>
@@ -931,6 +934,9 @@
       </c>
       <c r="R4">
         <v>6614.57</v>
+      </c>
+      <c r="S4" t="s">
+        <v>3</v>
       </c>
       <c r="T4">
         <v>6129.72</v>
@@ -1001,7 +1007,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <v>166321</v>
@@ -1120,7 +1126,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>166321</v>
@@ -1239,7 +1245,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>190301</v>
@@ -1358,7 +1364,7 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>190301</v>
@@ -1404,6 +1410,9 @@
       </c>
       <c r="R8">
         <v>8492.69</v>
+      </c>
+      <c r="S8" t="s">
+        <v>3</v>
       </c>
       <c r="T8">
         <v>6964.04</v>
@@ -1474,7 +1483,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>190301</v>
@@ -1593,7 +1602,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10">
         <v>190301</v>
@@ -1712,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <v>181792</v>
@@ -1831,7 +1840,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <v>181792</v>
@@ -1877,6 +1886,9 @@
       </c>
       <c r="R12">
         <v>9311.2900000000009</v>
+      </c>
+      <c r="S12" t="s">
+        <v>3</v>
       </c>
       <c r="U12">
         <v>8269.5</v>
@@ -1944,7 +1956,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <v>181792</v>
@@ -2063,7 +2075,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14">
         <v>181792</v>
@@ -2182,7 +2194,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15">
         <v>81844.100000000006</v>
@@ -2301,7 +2313,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16">
         <v>81844.100000000006</v>
@@ -2420,7 +2432,7 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <v>81844.100000000006</v>
@@ -2539,7 +2551,7 @@
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18">
         <v>81844.100000000006</v>
@@ -2658,7 +2670,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19">
         <v>120000</v>
@@ -2777,7 +2789,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20">
         <v>120000</v>
@@ -2890,7 +2902,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21">
         <v>120000</v>
@@ -3009,7 +3021,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22">
         <v>120000</v>
@@ -3128,7 +3140,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23">
         <v>310981</v>
@@ -3247,7 +3259,7 @@
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24">
         <v>310981</v>
@@ -3363,7 +3375,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25">
         <v>310981</v>
@@ -3482,7 +3494,7 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26">
         <v>310981</v>
@@ -3601,7 +3613,7 @@
         <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D27">
         <v>324148</v>
@@ -3720,7 +3732,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28">
         <v>324148</v>
@@ -3836,7 +3848,7 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29">
         <v>324148</v>
@@ -3955,7 +3967,7 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30">
         <v>324148</v>
@@ -4074,7 +4086,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D31">
         <v>181146</v>
@@ -4193,7 +4205,7 @@
         <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D32">
         <v>181146</v>
@@ -4239,6 +4251,9 @@
       </c>
       <c r="R32">
         <v>7382.67</v>
+      </c>
+      <c r="S32" t="s">
+        <v>3</v>
       </c>
       <c r="T32">
         <v>6163.62</v>
@@ -4309,7 +4324,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33">
         <v>181146</v>
@@ -4428,7 +4443,7 @@
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D34">
         <v>181146</v>
@@ -4541,136 +4556,136 @@
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D35">
-        <f>AVERAGE(D11,D15,D19,D23,D27,D31,AVERAGE(D3,D7))</f>
+        <f t="shared" ref="D35:AH35" si="0">AVERAGE(D11,D15,D19,D23,D27,D31,AVERAGE(D3,D7))</f>
         <v>196888.87142857144</v>
       </c>
       <c r="E35">
-        <f>AVERAGE(E11,E15,E19,E23,E27,E31,AVERAGE(E3,E7))</f>
+        <f t="shared" si="0"/>
         <v>145724.85714285713</v>
       </c>
       <c r="F35">
-        <f>AVERAGE(F11,F15,F19,F23,F27,F31,AVERAGE(F3,F7))</f>
+        <f t="shared" si="0"/>
         <v>107324.45714285714</v>
       </c>
       <c r="G35">
-        <f>AVERAGE(G11,G15,G19,G23,G27,G31,AVERAGE(G3,G7))</f>
+        <f t="shared" si="0"/>
         <v>85645.21428571429</v>
       </c>
       <c r="H35">
-        <f>AVERAGE(H11,H15,H19,H23,H27,H31,AVERAGE(H3,H7))</f>
+        <f t="shared" si="0"/>
         <v>68785.364285714284</v>
       </c>
       <c r="I35">
-        <f>AVERAGE(I11,I15,I19,I23,I27,I31,AVERAGE(I3,I7))</f>
+        <f t="shared" si="0"/>
         <v>50905.121428571423</v>
       </c>
       <c r="J35">
-        <f>AVERAGE(J11,J15,J19,J23,J27,J31,AVERAGE(J3,J7))</f>
+        <f t="shared" si="0"/>
         <v>39422.107142857145</v>
       </c>
       <c r="K35">
-        <f>AVERAGE(K11,K15,K19,K23,K27,K31,AVERAGE(K3,K7))</f>
+        <f t="shared" si="0"/>
         <v>32397.178571428569</v>
       </c>
       <c r="L35">
-        <f>AVERAGE(L11,L15,L19,L23,L27,L31,AVERAGE(L3,L7))</f>
+        <f t="shared" si="0"/>
         <v>28194.392857142859</v>
       </c>
       <c r="M35">
-        <f>AVERAGE(M11,M15,M19,M23,M27,M31,AVERAGE(M3,M7))</f>
+        <f t="shared" si="0"/>
         <v>24596.871428571427</v>
       </c>
       <c r="N35">
-        <f>AVERAGE(N11,N15,N19,N23,N27,N31,AVERAGE(N3,N7))</f>
+        <f t="shared" si="0"/>
         <v>21911.385714285716</v>
       </c>
       <c r="O35">
-        <f>AVERAGE(O11,O15,O19,O23,O27,O31,AVERAGE(O3,O7))</f>
+        <f t="shared" si="0"/>
         <v>19204.75</v>
       </c>
       <c r="P35">
-        <f>AVERAGE(P11,P15,P19,P23,P27,P31,AVERAGE(P3,P7))</f>
+        <f t="shared" si="0"/>
         <v>16993.471428571433</v>
       </c>
       <c r="Q35">
-        <f>AVERAGE(Q11,Q15,Q19,Q23,Q27,Q31,AVERAGE(Q3,Q7))</f>
+        <f t="shared" si="0"/>
         <v>10430.002857142857</v>
       </c>
       <c r="R35">
-        <f>AVERAGE(R11,R15,R19,R23,R27,R31,AVERAGE(R3,R7))</f>
+        <f t="shared" si="0"/>
         <v>7649.7285714285726</v>
       </c>
       <c r="S35">
-        <f>AVERAGE(S11,S15,S19,S23,S27,S31,AVERAGE(S3,S7))</f>
+        <f t="shared" si="0"/>
         <v>6223.6407142857133</v>
       </c>
       <c r="T35">
-        <f>AVERAGE(T11,T15,T19,T23,T27,T31,AVERAGE(T3,T7))</f>
+        <f t="shared" si="0"/>
         <v>5544.7408333333333</v>
       </c>
       <c r="U35">
-        <f>AVERAGE(U11,U15,U19,U23,U27,U31,AVERAGE(U3,U7))</f>
+        <f t="shared" si="0"/>
         <v>4990.9091666666664</v>
       </c>
       <c r="V35">
-        <f>AVERAGE(V11,V15,V19,V23,V27,V31,AVERAGE(V3,V7))</f>
+        <f t="shared" si="0"/>
         <v>4700.2219999999998</v>
       </c>
       <c r="W35">
-        <f>AVERAGE(W11,W15,W19,W23,W27,W31,AVERAGE(W3,W7))</f>
+        <f t="shared" si="0"/>
         <v>4426.3150000000005</v>
       </c>
       <c r="X35">
-        <f>AVERAGE(X11,X15,X19,X23,X27,X31,AVERAGE(X3,X7))</f>
+        <f t="shared" si="0"/>
         <v>4196.2420000000002</v>
       </c>
       <c r="Y35">
-        <f>AVERAGE(Y11,Y15,Y19,Y23,Y27,Y31,AVERAGE(Y3,Y7))</f>
+        <f t="shared" si="0"/>
         <v>4029.232</v>
       </c>
       <c r="Z35">
-        <f>AVERAGE(Z11,Z15,Z19,Z23,Z27,Z31,AVERAGE(Z3,Z7))</f>
+        <f t="shared" si="0"/>
         <v>3861.2340000000004</v>
       </c>
       <c r="AA35">
-        <f>AVERAGE(AA11,AA15,AA19,AA23,AA27,AA31,AVERAGE(AA3,AA7))</f>
+        <f t="shared" si="0"/>
         <v>3722.3199999999997</v>
       </c>
       <c r="AB35">
-        <f>AVERAGE(AB11,AB15,AB19,AB23,AB27,AB31,AVERAGE(AB3,AB7))</f>
+        <f t="shared" si="0"/>
         <v>3673.4209999999998</v>
       </c>
       <c r="AC35">
-        <f>AVERAGE(AC11,AC15,AC19,AC23,AC27,AC31,AVERAGE(AC3,AC7))</f>
+        <f t="shared" si="0"/>
         <v>3713.5209999999997</v>
       </c>
       <c r="AD35">
-        <f>AVERAGE(AD11,AD15,AD19,AD23,AD27,AD31,AVERAGE(AD3,AD7))</f>
+        <f t="shared" si="0"/>
         <v>3700.8870000000002</v>
       </c>
       <c r="AE35">
-        <f>AVERAGE(AE11,AE15,AE19,AE23,AE27,AE31,AVERAGE(AE3,AE7))</f>
+        <f t="shared" si="0"/>
         <v>3675.6320000000001</v>
       </c>
       <c r="AF35">
-        <f>AVERAGE(AF11,AF15,AF19,AF23,AF27,AF31,AVERAGE(AF3,AF7))</f>
+        <f t="shared" si="0"/>
         <v>3673.1390000000001</v>
       </c>
       <c r="AG35">
-        <f>AVERAGE(AG11,AG15,AG19,AG23,AG27,AG31,AVERAGE(AG3,AG7))</f>
+        <f t="shared" si="0"/>
         <v>3736.0674999999997</v>
       </c>
       <c r="AH35">
-        <f>AVERAGE(AH11,AH15,AH19,AH23,AH27,AH31,AVERAGE(AH3,AH7))</f>
+        <f t="shared" si="0"/>
         <v>4539.21</v>
       </c>
       <c r="AI35" t="s">
@@ -4691,136 +4706,135 @@
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36">
-        <f>AVERAGE(D12,D16,D20,D24,D28,D32,AVERAGE(D4,D8))</f>
+        <f t="shared" ref="D36:AH36" si="1">AVERAGE(D12,D16,D20,D24,D28,D32,AVERAGE(D4,D8))</f>
         <v>196888.87142857144</v>
       </c>
       <c r="E36">
-        <f>AVERAGE(E12,E16,E20,E24,E28,E32,AVERAGE(E4,E8))</f>
+        <f t="shared" si="1"/>
         <v>154441.28571428571</v>
       </c>
       <c r="F36">
-        <f>AVERAGE(F12,F16,F20,F24,F28,F32,AVERAGE(F4,F8))</f>
+        <f t="shared" si="1"/>
         <v>115399.32857142857</v>
       </c>
       <c r="G36">
-        <f>AVERAGE(G12,G16,G20,G24,G28,G32,AVERAGE(G4,G8))</f>
+        <f t="shared" si="1"/>
         <v>92991.664285714287</v>
       </c>
       <c r="H36">
-        <f>AVERAGE(H12,H16,H20,H24,H28,H32,AVERAGE(H4,H8))</f>
+        <f t="shared" si="1"/>
         <v>74232.53571428571</v>
       </c>
       <c r="I36">
-        <f>AVERAGE(I12,I16,I20,I24,I28,I32,AVERAGE(I4,I8))</f>
+        <f t="shared" si="1"/>
         <v>53431.607142857145</v>
       </c>
       <c r="J36">
-        <f>AVERAGE(J12,J16,J20,J24,J28,J32,AVERAGE(J4,J8))</f>
+        <f t="shared" si="1"/>
         <v>42975.4</v>
       </c>
       <c r="K36">
-        <f>AVERAGE(K12,K16,K20,K24,K28,K32,AVERAGE(K4,K8))</f>
+        <f t="shared" si="1"/>
         <v>36492.85</v>
       </c>
       <c r="L36">
-        <f>AVERAGE(L12,L16,L20,L24,L28,L32,AVERAGE(L4,L8))</f>
+        <f t="shared" si="1"/>
         <v>31530.292857142857</v>
       </c>
       <c r="M36">
-        <f>AVERAGE(M12,M16,M20,M24,M28,M32,AVERAGE(M4,M8))</f>
+        <f t="shared" si="1"/>
         <v>26109.271428571428</v>
       </c>
       <c r="N36">
-        <f>AVERAGE(N12,N16,N20,N24,N28,N32,AVERAGE(N4,N8))</f>
+        <f t="shared" si="1"/>
         <v>23872.014285714286</v>
       </c>
       <c r="O36">
-        <f>AVERAGE(O12,O16,O20,O24,O28,O32,AVERAGE(O4,O8))</f>
+        <f t="shared" si="1"/>
         <v>22338.864285714284</v>
       </c>
       <c r="P36">
-        <f>AVERAGE(P12,P16,P20,P24,P28,P32,AVERAGE(P4,P8))</f>
+        <f t="shared" si="1"/>
         <v>20961.842857142856</v>
       </c>
       <c r="Q36">
-        <f>AVERAGE(Q12,Q16,Q20,Q24,Q28,Q32,AVERAGE(Q4,Q8))</f>
+        <f t="shared" si="1"/>
         <v>12521.85</v>
       </c>
       <c r="R36">
-        <f>AVERAGE(R12,R16,R20,R24,R28,R32,AVERAGE(R4,R8))</f>
+        <f t="shared" si="1"/>
         <v>9033.7849999999999</v>
       </c>
-      <c r="S36" t="e">
-        <f>AVERAGE(S12,S16,S20,S24,S28,S32,AVERAGE(S4,S8))</f>
-        <v>#DIV/0!</v>
+      <c r="S36" t="s">
+        <v>3</v>
       </c>
       <c r="T36">
-        <f>AVERAGE(T12,T16,T20,T24,T28,T32,AVERAGE(T4,T8))</f>
+        <f t="shared" si="1"/>
         <v>6417.2559999999994</v>
       </c>
       <c r="U36">
-        <f>AVERAGE(U12,U16,U20,U24,U28,U32,AVERAGE(U4,U8))</f>
+        <f t="shared" si="1"/>
         <v>6650.9566666666678</v>
       </c>
       <c r="V36">
-        <f>AVERAGE(V12,V16,V20,V24,V28,V32,AVERAGE(V4,V8))</f>
+        <f t="shared" si="1"/>
         <v>6408.5241666666661</v>
       </c>
       <c r="W36">
-        <f>AVERAGE(W12,W16,W20,W24,W28,W32,AVERAGE(W4,W8))</f>
+        <f t="shared" si="1"/>
         <v>6232.0741666666654</v>
       </c>
       <c r="X36">
-        <f>AVERAGE(X12,X16,X20,X24,X28,X32,AVERAGE(X4,X8))</f>
+        <f t="shared" si="1"/>
         <v>5959.3041666666677</v>
       </c>
       <c r="Y36">
-        <f>AVERAGE(Y12,Y16,Y20,Y24,Y28,Y32,AVERAGE(Y4,Y8))</f>
+        <f t="shared" si="1"/>
         <v>5609.0074999999997</v>
       </c>
       <c r="Z36">
-        <f>AVERAGE(Z12,Z16,Z20,Z24,Z28,Z32,AVERAGE(Z4,Z8))</f>
+        <f t="shared" si="1"/>
         <v>5347.6675000000005</v>
       </c>
       <c r="AA36">
-        <f>AVERAGE(AA12,AA16,AA20,AA24,AA28,AA32,AVERAGE(AA4,AA8))</f>
+        <f t="shared" si="1"/>
         <v>5139.225833333333</v>
       </c>
       <c r="AB36">
-        <f>AVERAGE(AB12,AB16,AB20,AB24,AB28,AB32,AVERAGE(AB4,AB8))</f>
+        <f t="shared" si="1"/>
         <v>4989.0708333333332</v>
       </c>
       <c r="AC36">
-        <f>AVERAGE(AC12,AC16,AC20,AC24,AC28,AC32,AVERAGE(AC4,AC8))</f>
+        <f t="shared" si="1"/>
         <v>4886.4350000000004</v>
       </c>
       <c r="AD36">
-        <f>AVERAGE(AD12,AD16,AD20,AD24,AD28,AD32,AVERAGE(AD4,AD8))</f>
+        <f t="shared" si="1"/>
         <v>4806.5700000000006</v>
       </c>
       <c r="AE36">
-        <f>AVERAGE(AE12,AE16,AE20,AE24,AE28,AE32,AVERAGE(AE4,AE8))</f>
+        <f t="shared" si="1"/>
         <v>4726.1125000000002</v>
       </c>
       <c r="AF36">
-        <f>AVERAGE(AF12,AF16,AF20,AF24,AF28,AF32,AVERAGE(AF4,AF8))</f>
+        <f t="shared" si="1"/>
         <v>4720.876666666667</v>
       </c>
       <c r="AG36">
-        <f>AVERAGE(AG12,AG16,AG20,AG24,AG28,AG32,AVERAGE(AG4,AG8))</f>
+        <f t="shared" si="1"/>
         <v>4716.72</v>
       </c>
       <c r="AH36">
-        <f>AVERAGE(AH12,AH16,AH20,AH24,AH28,AH32,AVERAGE(AH4,AH8))</f>
+        <f t="shared" si="1"/>
         <v>4846.2441666666664</v>
       </c>
       <c r="AI36">
@@ -4844,136 +4858,136 @@
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D37">
-        <f>AVERAGE(D13,D17,D21,D25,D29,D33,AVERAGE(D5,D9))</f>
+        <f t="shared" ref="D37:AH37" si="2">AVERAGE(D13,D17,D21,D25,D29,D33,AVERAGE(D5,D9))</f>
         <v>196888.87142857144</v>
       </c>
       <c r="E37">
-        <f>AVERAGE(E13,E17,E21,E25,E29,E33,AVERAGE(E5,E9))</f>
+        <f t="shared" si="2"/>
         <v>140595.22857142857</v>
       </c>
       <c r="F37">
-        <f>AVERAGE(F13,F17,F21,F25,F29,F33,AVERAGE(F5,F9))</f>
+        <f t="shared" si="2"/>
         <v>105145.41428571429</v>
       </c>
       <c r="G37">
-        <f>AVERAGE(G13,G17,G21,G25,G29,G33,AVERAGE(G5,G9))</f>
+        <f t="shared" si="2"/>
         <v>83181.835714285713</v>
       </c>
       <c r="H37">
-        <f>AVERAGE(H13,H17,H21,H25,H29,H33,AVERAGE(H5,H9))</f>
+        <f t="shared" si="2"/>
         <v>65105.92857142858</v>
       </c>
       <c r="I37">
-        <f>AVERAGE(I13,I17,I21,I25,I29,I33,AVERAGE(I5,I9))</f>
+        <f t="shared" si="2"/>
         <v>46900.214285714283</v>
       </c>
       <c r="J37">
-        <f>AVERAGE(J13,J17,J21,J25,J29,J33,AVERAGE(J5,J9))</f>
+        <f t="shared" si="2"/>
         <v>35696.428571428572</v>
       </c>
       <c r="K37">
-        <f>AVERAGE(K13,K17,K21,K25,K29,K33,AVERAGE(K5,K9))</f>
+        <f t="shared" si="2"/>
         <v>28034.028571428575</v>
       </c>
       <c r="L37">
-        <f>AVERAGE(L13,L17,L21,L25,L29,L33,AVERAGE(L5,L9))</f>
+        <f t="shared" si="2"/>
         <v>24346.064285714288</v>
       </c>
       <c r="M37">
-        <f>AVERAGE(M13,M17,M21,M25,M29,M33,AVERAGE(M5,M9))</f>
+        <f t="shared" si="2"/>
         <v>21231.799999999996</v>
       </c>
       <c r="N37">
-        <f>AVERAGE(N13,N17,N21,N25,N29,N33,AVERAGE(N5,N9))</f>
+        <f t="shared" si="2"/>
         <v>19248.82857142857</v>
       </c>
       <c r="O37">
-        <f>AVERAGE(O13,O17,O21,O25,O29,O33,AVERAGE(O5,O9))</f>
+        <f t="shared" si="2"/>
         <v>17452.67142857143</v>
       </c>
       <c r="P37">
-        <f>AVERAGE(P13,P17,P21,P25,P29,P33,AVERAGE(P5,P9))</f>
+        <f t="shared" si="2"/>
         <v>15862.921428571428</v>
       </c>
       <c r="Q37">
-        <f>AVERAGE(Q13,Q17,Q21,Q25,Q29,Q33,AVERAGE(Q5,Q9))</f>
+        <f t="shared" si="2"/>
         <v>10101.775714285714</v>
       </c>
       <c r="R37">
-        <f>AVERAGE(R13,R17,R21,R25,R29,R33,AVERAGE(R5,R9))</f>
+        <f t="shared" si="2"/>
         <v>7580.5885714285705</v>
       </c>
       <c r="S37">
-        <f>AVERAGE(S13,S17,S21,S25,S29,S33,AVERAGE(S5,S9))</f>
+        <f t="shared" si="2"/>
         <v>5911.0524999999989</v>
       </c>
       <c r="T37">
-        <f>AVERAGE(T13,T17,T21,T25,T29,T33,AVERAGE(T5,T9))</f>
+        <f t="shared" si="2"/>
         <v>5293.9691666666668</v>
       </c>
       <c r="U37">
-        <f>AVERAGE(U13,U17,U21,U25,U29,U33,AVERAGE(U5,U9))</f>
+        <f t="shared" si="2"/>
         <v>4868.0016666666661</v>
       </c>
       <c r="V37">
-        <f>AVERAGE(V13,V17,V21,V25,V29,V33,AVERAGE(V5,V9))</f>
+        <f t="shared" si="2"/>
         <v>4575.150833333334</v>
       </c>
       <c r="W37">
-        <f>AVERAGE(W13,W17,W21,W25,W29,W33,AVERAGE(W5,W9))</f>
+        <f t="shared" si="2"/>
         <v>4366.8225000000011</v>
       </c>
       <c r="X37">
-        <f>AVERAGE(X13,X17,X21,X25,X29,X33,AVERAGE(X5,X9))</f>
+        <f t="shared" si="2"/>
         <v>4232.0091666666667</v>
       </c>
       <c r="Y37">
-        <f>AVERAGE(Y13,Y17,Y21,Y25,Y29,Y33,AVERAGE(Y5,Y9))</f>
+        <f t="shared" si="2"/>
         <v>4083.7874999999999</v>
       </c>
       <c r="Z37">
-        <f>AVERAGE(Z13,Z17,Z21,Z25,Z29,Z33,AVERAGE(Z5,Z9))</f>
+        <f t="shared" si="2"/>
         <v>3905.9041666666672</v>
       </c>
       <c r="AA37">
-        <f>AVERAGE(AA13,AA17,AA21,AA25,AA29,AA33,AVERAGE(AA5,AA9))</f>
+        <f t="shared" si="2"/>
         <v>3917.3510000000001</v>
       </c>
       <c r="AB37">
-        <f>AVERAGE(AB13,AB17,AB21,AB25,AB29,AB33,AVERAGE(AB5,AB9))</f>
+        <f t="shared" si="2"/>
         <v>3871.2519999999995</v>
       </c>
       <c r="AC37">
-        <f>AVERAGE(AC13,AC17,AC21,AC25,AC29,AC33,AVERAGE(AC5,AC9))</f>
+        <f t="shared" si="2"/>
         <v>3847.3340000000003</v>
       </c>
       <c r="AD37">
-        <f>AVERAGE(AD13,AD17,AD21,AD25,AD29,AD33,AVERAGE(AD5,AD9))</f>
+        <f t="shared" si="2"/>
         <v>3777.7510000000002</v>
       </c>
       <c r="AE37">
-        <f>AVERAGE(AE13,AE17,AE21,AE25,AE29,AE33,AVERAGE(AE5,AE9))</f>
+        <f t="shared" si="2"/>
         <v>3727.65</v>
       </c>
       <c r="AF37">
-        <f>AVERAGE(AF13,AF17,AF21,AF25,AF29,AF33,AVERAGE(AF5,AF9))</f>
+        <f t="shared" si="2"/>
         <v>3767.2200000000003</v>
       </c>
       <c r="AG37">
-        <f>AVERAGE(AG13,AG17,AG21,AG25,AG29,AG33,AVERAGE(AG5,AG9))</f>
+        <f t="shared" si="2"/>
         <v>3722.7987499999999</v>
       </c>
       <c r="AH37">
-        <f>AVERAGE(AH13,AH17,AH21,AH25,AH29,AH33,AVERAGE(AH5,AH9))</f>
+        <f t="shared" si="2"/>
         <v>3983.14</v>
       </c>
       <c r="AI37">
@@ -4995,128 +5009,128 @@
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
       </c>
       <c r="C38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D38">
-        <f>AVERAGE(D14,D18,D22,D26,D30,D34,AVERAGE(D6,D10))</f>
+        <f t="shared" ref="D38:AF38" si="3">AVERAGE(D14,D18,D22,D26,D30,D34,AVERAGE(D6,D10))</f>
         <v>196888.87142857144</v>
       </c>
       <c r="E38">
-        <f>AVERAGE(E14,E18,E22,E26,E30,E34,AVERAGE(E6,E10))</f>
+        <f t="shared" si="3"/>
         <v>162414.08571428573</v>
       </c>
       <c r="F38">
-        <f>AVERAGE(F14,F18,F22,F26,F30,F34,AVERAGE(F6,F10))</f>
+        <f t="shared" si="3"/>
         <v>121619.14285714286</v>
       </c>
       <c r="G38">
-        <f>AVERAGE(G14,G18,G22,G26,G30,G34,AVERAGE(G6,G10))</f>
+        <f t="shared" si="3"/>
         <v>98423.585714285713</v>
       </c>
       <c r="H38">
-        <f>AVERAGE(H14,H18,H22,H26,H30,H34,AVERAGE(H6,H10))</f>
+        <f t="shared" si="3"/>
         <v>80004.457142857136</v>
       </c>
       <c r="I38">
-        <f>AVERAGE(I14,I18,I22,I26,I30,I34,AVERAGE(I6,I10))</f>
+        <f t="shared" si="3"/>
         <v>57712.085714285713</v>
       </c>
       <c r="J38">
-        <f>AVERAGE(J14,J18,J22,J26,J30,J34,AVERAGE(J6,J10))</f>
+        <f t="shared" si="3"/>
         <v>45420.357142857145</v>
       </c>
       <c r="K38">
-        <f>AVERAGE(K14,K18,K22,K26,K30,K34,AVERAGE(K6,K10))</f>
+        <f t="shared" si="3"/>
         <v>38380.400000000001</v>
       </c>
       <c r="L38">
-        <f>AVERAGE(L14,L18,L22,L26,L30,L34,AVERAGE(L6,L10))</f>
+        <f t="shared" si="3"/>
         <v>34223.235714285714</v>
       </c>
       <c r="M38">
-        <f>AVERAGE(M14,M18,M22,M26,M30,M34,AVERAGE(M6,M10))</f>
+        <f t="shared" si="3"/>
         <v>29027.242857142857</v>
       </c>
       <c r="N38">
-        <f>AVERAGE(N14,N18,N22,N26,N30,N34,AVERAGE(N6,N10))</f>
+        <f t="shared" si="3"/>
         <v>24144.342857142856</v>
       </c>
       <c r="O38">
-        <f>AVERAGE(O14,O18,O22,O26,O30,O34,AVERAGE(O6,O10))</f>
+        <f t="shared" si="3"/>
         <v>21165.078571428574</v>
       </c>
       <c r="P38">
-        <f>AVERAGE(P14,P18,P22,P26,P30,P34,AVERAGE(P6,P10))</f>
+        <f t="shared" si="3"/>
         <v>19698.685714285712</v>
       </c>
       <c r="Q38">
-        <f>AVERAGE(Q14,Q18,Q22,Q26,Q30,Q34,AVERAGE(Q6,Q10))</f>
+        <f t="shared" si="3"/>
         <v>11703.011428571428</v>
       </c>
       <c r="R38">
-        <f>AVERAGE(R14,R18,R22,R26,R30,R34,AVERAGE(R6,R10))</f>
+        <f t="shared" si="3"/>
         <v>9118.1164285714294</v>
       </c>
       <c r="S38">
-        <f>AVERAGE(S14,S18,S22,S26,S30,S34,AVERAGE(S6,S10))</f>
+        <f t="shared" si="3"/>
         <v>7030.232857142857</v>
       </c>
       <c r="T38">
-        <f>AVERAGE(T14,T18,T22,T26,T30,T34,AVERAGE(T6,T10))</f>
+        <f t="shared" si="3"/>
         <v>5785.5291666666672</v>
       </c>
       <c r="U38">
-        <f>AVERAGE(U14,U18,U22,U26,U30,U34,AVERAGE(U6,U10))</f>
+        <f t="shared" si="3"/>
         <v>5103.2533333333331</v>
       </c>
       <c r="V38">
-        <f>AVERAGE(V14,V18,V22,V26,V30,V34,AVERAGE(V6,V10))</f>
+        <f t="shared" si="3"/>
         <v>4779.8750000000009</v>
       </c>
       <c r="W38">
-        <f>AVERAGE(W14,W18,W22,W26,W30,W34,AVERAGE(W6,W10))</f>
+        <f t="shared" si="3"/>
         <v>4476.774166666667</v>
       </c>
       <c r="X38">
-        <f>AVERAGE(X14,X18,X22,X26,X30,X34,AVERAGE(X6,X10))</f>
+        <f t="shared" si="3"/>
         <v>4208.1100000000006</v>
       </c>
       <c r="Y38">
-        <f>AVERAGE(Y14,Y18,Y22,Y26,Y30,Y34,AVERAGE(Y6,Y10))</f>
+        <f t="shared" si="3"/>
         <v>3887.7374999999997</v>
       </c>
       <c r="Z38">
-        <f>AVERAGE(Z14,Z18,Z22,Z26,Z30,Z34,AVERAGE(Z6,Z10))</f>
+        <f t="shared" si="3"/>
         <v>3763.4769999999999</v>
       </c>
       <c r="AA38">
-        <f>AVERAGE(AA14,AA18,AA22,AA26,AA30,AA34,AVERAGE(AA6,AA10))</f>
+        <f t="shared" si="3"/>
         <v>3538.7979999999998</v>
       </c>
       <c r="AB38">
-        <f>AVERAGE(AB14,AB18,AB22,AB26,AB30,AB34,AVERAGE(AB6,AB10))</f>
+        <f t="shared" si="3"/>
         <v>3435.9550000000004</v>
       </c>
       <c r="AC38">
-        <f>AVERAGE(AC14,AC18,AC22,AC26,AC30,AC34,AVERAGE(AC6,AC10))</f>
+        <f t="shared" si="3"/>
         <v>3368.30125</v>
       </c>
       <c r="AD38">
-        <f>AVERAGE(AD14,AD18,AD22,AD26,AD30,AD34,AVERAGE(AD6,AD10))</f>
+        <f t="shared" si="3"/>
         <v>3335.5012500000003</v>
       </c>
       <c r="AE38">
-        <f>AVERAGE(AE14,AE18,AE22,AE26,AE30,AE34,AVERAGE(AE6,AE10))</f>
+        <f t="shared" si="3"/>
         <v>3175.5262499999999</v>
       </c>
       <c r="AF38">
-        <f>AVERAGE(AF14,AF18,AF22,AF26,AF30,AF34,AVERAGE(AF6,AF10))</f>
+        <f t="shared" si="3"/>
         <v>3069.5662499999999</v>
       </c>
       <c r="AG38" t="s">
@@ -5138,6 +5152,482 @@
         <v>3</v>
       </c>
       <c r="AM38" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39">
+        <v>196890</v>
+      </c>
+      <c r="E39">
+        <v>145724.28571428571</v>
+      </c>
+      <c r="F39">
+        <v>107324.57142857143</v>
+      </c>
+      <c r="G39">
+        <v>85645.28571428571</v>
+      </c>
+      <c r="H39">
+        <v>68785.28571428571</v>
+      </c>
+      <c r="I39">
+        <v>50905.142857142855</v>
+      </c>
+      <c r="J39">
+        <v>39422.285714285717</v>
+      </c>
+      <c r="K39">
+        <v>32397.142857142859</v>
+      </c>
+      <c r="L39">
+        <v>28194.428571428572</v>
+      </c>
+      <c r="M39">
+        <v>24597</v>
+      </c>
+      <c r="N39">
+        <v>21911.428571428572</v>
+      </c>
+      <c r="O39">
+        <v>19204.714285714286</v>
+      </c>
+      <c r="P39">
+        <v>16993.428571428572</v>
+      </c>
+      <c r="Q39">
+        <v>10430</v>
+      </c>
+      <c r="R39">
+        <v>7649.7428571428563</v>
+      </c>
+      <c r="S39">
+        <v>6223.6285714285714</v>
+      </c>
+      <c r="T39">
+        <v>5544.7333333333336</v>
+      </c>
+      <c r="U39">
+        <v>4990.9000000000005</v>
+      </c>
+      <c r="V39">
+        <v>4700.2199999999993</v>
+      </c>
+      <c r="W39">
+        <v>4426.32</v>
+      </c>
+      <c r="X39">
+        <v>4196.24</v>
+      </c>
+      <c r="Y39">
+        <v>4029.2400000000002</v>
+      </c>
+      <c r="Z39">
+        <v>3861.2400000000002</v>
+      </c>
+      <c r="AA39">
+        <v>3722.3199999999997</v>
+      </c>
+      <c r="AB39">
+        <v>3673.4199999999996</v>
+      </c>
+      <c r="AC39">
+        <v>3713.5199999999995</v>
+      </c>
+      <c r="AD39">
+        <v>3700.9</v>
+      </c>
+      <c r="AE39">
+        <v>3675.6400000000003</v>
+      </c>
+      <c r="AF39">
+        <v>3673.1400000000003</v>
+      </c>
+      <c r="AG39">
+        <v>3736.0749999999998</v>
+      </c>
+      <c r="AH39">
+        <v>4539.2</v>
+      </c>
+      <c r="AI39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40">
+        <v>196890</v>
+      </c>
+      <c r="E40">
+        <v>154441.42857142858</v>
+      </c>
+      <c r="F40">
+        <v>115399.42857142857</v>
+      </c>
+      <c r="G40">
+        <v>92991.857142857145</v>
+      </c>
+      <c r="H40">
+        <v>74232.71428571429</v>
+      </c>
+      <c r="I40">
+        <v>53431.571428571428</v>
+      </c>
+      <c r="J40">
+        <v>42975.428571428572</v>
+      </c>
+      <c r="K40">
+        <v>36493</v>
+      </c>
+      <c r="L40">
+        <v>31530.428571428572</v>
+      </c>
+      <c r="M40">
+        <v>26109.285714285714</v>
+      </c>
+      <c r="N40">
+        <v>23872</v>
+      </c>
+      <c r="O40">
+        <v>22338.857142857141</v>
+      </c>
+      <c r="P40">
+        <v>20961.857142857141</v>
+      </c>
+      <c r="Q40">
+        <v>12521.857142857143</v>
+      </c>
+      <c r="R40">
+        <v>8848.6857142857152</v>
+      </c>
+      <c r="S40" t="s">
+        <v>3</v>
+      </c>
+      <c r="T40">
+        <v>7178.6500000000005</v>
+      </c>
+      <c r="U40">
+        <v>6650.95</v>
+      </c>
+      <c r="V40">
+        <v>6408.5166666666664</v>
+      </c>
+      <c r="W40">
+        <v>6232.0999999999995</v>
+      </c>
+      <c r="X40">
+        <v>5959.3166666666666</v>
+      </c>
+      <c r="Y40">
+        <v>5609.0333333333328</v>
+      </c>
+      <c r="Z40">
+        <v>5347.6500000000005</v>
+      </c>
+      <c r="AA40">
+        <v>5139.2333333333336</v>
+      </c>
+      <c r="AB40">
+        <v>4989.0666666666666</v>
+      </c>
+      <c r="AC40">
+        <v>4886.45</v>
+      </c>
+      <c r="AD40">
+        <v>4806.5666666666666</v>
+      </c>
+      <c r="AE40">
+        <v>4726.1166666666668</v>
+      </c>
+      <c r="AF40">
+        <v>4720.8833333333332</v>
+      </c>
+      <c r="AG40">
+        <v>4716.7166666666662</v>
+      </c>
+      <c r="AH40">
+        <v>4846.25</v>
+      </c>
+      <c r="AI40">
+        <v>5233.88</v>
+      </c>
+      <c r="AJ40">
+        <v>4906.4250000000002</v>
+      </c>
+      <c r="AK40">
+        <v>5190.6499999999996</v>
+      </c>
+      <c r="AL40" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41">
+        <v>196890</v>
+      </c>
+      <c r="E41">
+        <v>140595.28571428571</v>
+      </c>
+      <c r="F41">
+        <v>105145.57142857143</v>
+      </c>
+      <c r="G41">
+        <v>83181.857142857145</v>
+      </c>
+      <c r="H41">
+        <v>65106</v>
+      </c>
+      <c r="I41">
+        <v>46900.142857142855</v>
+      </c>
+      <c r="J41">
+        <v>35696.428571428572</v>
+      </c>
+      <c r="K41">
+        <v>28034.142857142859</v>
+      </c>
+      <c r="L41">
+        <v>24346</v>
+      </c>
+      <c r="M41">
+        <v>21231.857142857141</v>
+      </c>
+      <c r="N41">
+        <v>19248.714285714286</v>
+      </c>
+      <c r="O41">
+        <v>17452.714285714286</v>
+      </c>
+      <c r="P41">
+        <v>15863</v>
+      </c>
+      <c r="Q41">
+        <v>10101.785714285714</v>
+      </c>
+      <c r="R41">
+        <v>7580.5999999999995</v>
+      </c>
+      <c r="S41">
+        <v>5911.05</v>
+      </c>
+      <c r="T41">
+        <v>5293.9666666666662</v>
+      </c>
+      <c r="U41">
+        <v>4868</v>
+      </c>
+      <c r="V41">
+        <v>4575.1333333333332</v>
+      </c>
+      <c r="W41">
+        <v>4366.833333333333</v>
+      </c>
+      <c r="X41">
+        <v>4232.0166666666664</v>
+      </c>
+      <c r="Y41">
+        <v>4228.88</v>
+      </c>
+      <c r="Z41">
+        <v>4068.72</v>
+      </c>
+      <c r="AA41">
+        <v>3917.3599999999997</v>
+      </c>
+      <c r="AB41">
+        <v>3871.2599999999998</v>
+      </c>
+      <c r="AC41">
+        <v>3847.34</v>
+      </c>
+      <c r="AD41">
+        <v>3777.7599999999998</v>
+      </c>
+      <c r="AE41">
+        <v>3727.66</v>
+      </c>
+      <c r="AF41">
+        <v>3767.2249999999999</v>
+      </c>
+      <c r="AG41">
+        <v>3722.8</v>
+      </c>
+      <c r="AH41">
+        <v>3983.1333333333332</v>
+      </c>
+      <c r="AI41">
+        <v>3227.2</v>
+      </c>
+      <c r="AJ41" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK41" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL41" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42">
+        <v>196890</v>
+      </c>
+      <c r="E42">
+        <v>162414.28571428571</v>
+      </c>
+      <c r="F42">
+        <v>121619.28571428571</v>
+      </c>
+      <c r="G42">
+        <v>98423.571428571435</v>
+      </c>
+      <c r="H42">
+        <v>80004.428571428565</v>
+      </c>
+      <c r="I42">
+        <v>57712.142857142855</v>
+      </c>
+      <c r="J42">
+        <v>45420.285714285717</v>
+      </c>
+      <c r="K42">
+        <v>38380.428571428572</v>
+      </c>
+      <c r="L42">
+        <v>34223.285714285717</v>
+      </c>
+      <c r="M42">
+        <v>29027.428571428572</v>
+      </c>
+      <c r="N42">
+        <v>24144.285714285714</v>
+      </c>
+      <c r="O42">
+        <v>21165.142857142859</v>
+      </c>
+      <c r="P42">
+        <v>19698.571428571428</v>
+      </c>
+      <c r="Q42">
+        <v>11703.014285714287</v>
+      </c>
+      <c r="R42">
+        <v>9118.1142857142859</v>
+      </c>
+      <c r="S42">
+        <v>7030.2285714285708</v>
+      </c>
+      <c r="T42">
+        <v>5785.5333333333328</v>
+      </c>
+      <c r="U42">
+        <v>5103.25</v>
+      </c>
+      <c r="V42">
+        <v>4779.8666666666668</v>
+      </c>
+      <c r="W42">
+        <v>4476.7666666666664</v>
+      </c>
+      <c r="X42">
+        <v>4208.1166666666668</v>
+      </c>
+      <c r="Y42">
+        <v>3887.75</v>
+      </c>
+      <c r="Z42">
+        <v>3763.4800000000005</v>
+      </c>
+      <c r="AA42">
+        <v>3538.8</v>
+      </c>
+      <c r="AB42">
+        <v>3435.95</v>
+      </c>
+      <c r="AC42">
+        <v>3368.3</v>
+      </c>
+      <c r="AD42">
+        <v>3335.5</v>
+      </c>
+      <c r="AE42">
+        <v>3175.5250000000001</v>
+      </c>
+      <c r="AF42">
+        <v>3069.5749999999998</v>
+      </c>
+      <c r="AG42">
+        <v>3358.98</v>
+      </c>
+      <c r="AH42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM42" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More Curcio data checking and provenance
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/data/Curcio_1990_JCompNeurol_HumanPhotoreceptorTopography/DENSITY8_cones_resorted_computedAverage.xlsx
+++ b/data/Curcio_1990_JCompNeurol_HumanPhotoreceptorTopography/DENSITY8_cones_resorted_computedAverage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="440" windowWidth="30160" windowHeight="20360" tabRatio="500"/>
+    <workbookView xWindow="1420" yWindow="440" windowWidth="49780" windowHeight="28360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DENSITY8_cones_resorted" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="58">
   <si>
     <t>ALL</t>
   </si>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T10" workbookViewId="0">
-      <selection activeCell="AG47" sqref="AG47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AE50" sqref="AE50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5018,7 +5018,7 @@
         <v>14</v>
       </c>
       <c r="D38">
-        <f t="shared" ref="D38:AF38" si="3">AVERAGE(D14,D18,D22,D26,D30,D34,AVERAGE(D6,D10))</f>
+        <f t="shared" ref="D38:AG38" si="3">AVERAGE(D14,D18,D22,D26,D30,D34,AVERAGE(D6,D10))</f>
         <v>196888.87142857144</v>
       </c>
       <c r="E38">
@@ -5133,8 +5133,9 @@
         <f t="shared" si="3"/>
         <v>3069.5662499999999</v>
       </c>
-      <c r="AG38" t="s">
-        <v>3</v>
+      <c r="AG38">
+        <f>AVERAGE(AG14,AG18,AG22,AG26,AG30,AG34,)</f>
+        <v>2239.3200000000002</v>
       </c>
       <c r="AH38" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Remade the data files with greater unit specificity
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/data/Curcio_1990_JCompNeurol_HumanPhotoreceptorTopography/DENSITY8_cones_resorted_computedAverage.xlsx
+++ b/data/Curcio_1990_JCompNeurol_HumanPhotoreceptorTopography/DENSITY8_cones_resorted_computedAverage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="440" windowWidth="49780" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="5820" yWindow="3580" windowWidth="39320" windowHeight="24680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DENSITY8_cones_resorted" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>support</t>
   </si>
   <si>
-    <t>degrees</t>
-  </si>
-  <si>
     <t>Subject</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>reportedAverage</t>
+  </si>
+  <si>
+    <t>retinalDegree</t>
   </si>
 </sst>
 </file>
@@ -518,128 +518,128 @@
   <dimension ref="A1:AM42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE50" sqref="AE50"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>30</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>31</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>34</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>35</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>36</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>37</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>38</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>39</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>40</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>42</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>43</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>45</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>46</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>47</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>48</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>49</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>50</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>51</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>52</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>53</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>54</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.2">
@@ -650,7 +650,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4556,7 +4556,7 @@
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" t="s">
         <v>2</v>
@@ -4706,7 +4706,7 @@
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B36" t="s">
         <v>4</v>
@@ -4858,7 +4858,7 @@
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
@@ -5009,7 +5009,7 @@
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -5018,7 +5018,7 @@
         <v>14</v>
       </c>
       <c r="D38">
-        <f t="shared" ref="D38:AG38" si="3">AVERAGE(D14,D18,D22,D26,D30,D34,AVERAGE(D6,D10))</f>
+        <f t="shared" ref="D38:AF38" si="3">AVERAGE(D14,D18,D22,D26,D30,D34,AVERAGE(D6,D10))</f>
         <v>196888.87142857144</v>
       </c>
       <c r="E38">
@@ -5158,7 +5158,7 @@
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
@@ -5277,7 +5277,7 @@
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
         <v>4</v>
@@ -5396,7 +5396,7 @@
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
@@ -5515,7 +5515,7 @@
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Working on the data validation
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/data/Curcio_1990_JCompNeurol_HumanPhotoreceptorTopography/DENSITY8_cones_resorted_computedAverage.xlsx
+++ b/data/Curcio_1990_JCompNeurol_HumanPhotoreceptorTopography/DENSITY8_cones_resorted_computedAverage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="3580" windowWidth="39320" windowHeight="24680" tabRatio="500"/>
+    <workbookView xWindow="1020" yWindow="440" windowWidth="27780" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DENSITY8_cones_resorted" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="57">
   <si>
     <t>ALL</t>
   </si>
@@ -195,9 +195,6 @@
   </si>
   <si>
     <t>computedAverage</t>
-  </si>
-  <si>
-    <t>reportedAverage</t>
   </si>
   <si>
     <t>retinalDegree</t>
@@ -515,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM42"/>
+  <dimension ref="A1:AM38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,7 +647,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -5153,482 +5150,6 @@
         <v>3</v>
       </c>
       <c r="AM38" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39">
-        <v>196890</v>
-      </c>
-      <c r="E39">
-        <v>145724.28571428571</v>
-      </c>
-      <c r="F39">
-        <v>107324.57142857143</v>
-      </c>
-      <c r="G39">
-        <v>85645.28571428571</v>
-      </c>
-      <c r="H39">
-        <v>68785.28571428571</v>
-      </c>
-      <c r="I39">
-        <v>50905.142857142855</v>
-      </c>
-      <c r="J39">
-        <v>39422.285714285717</v>
-      </c>
-      <c r="K39">
-        <v>32397.142857142859</v>
-      </c>
-      <c r="L39">
-        <v>28194.428571428572</v>
-      </c>
-      <c r="M39">
-        <v>24597</v>
-      </c>
-      <c r="N39">
-        <v>21911.428571428572</v>
-      </c>
-      <c r="O39">
-        <v>19204.714285714286</v>
-      </c>
-      <c r="P39">
-        <v>16993.428571428572</v>
-      </c>
-      <c r="Q39">
-        <v>10430</v>
-      </c>
-      <c r="R39">
-        <v>7649.7428571428563</v>
-      </c>
-      <c r="S39">
-        <v>6223.6285714285714</v>
-      </c>
-      <c r="T39">
-        <v>5544.7333333333336</v>
-      </c>
-      <c r="U39">
-        <v>4990.9000000000005</v>
-      </c>
-      <c r="V39">
-        <v>4700.2199999999993</v>
-      </c>
-      <c r="W39">
-        <v>4426.32</v>
-      </c>
-      <c r="X39">
-        <v>4196.24</v>
-      </c>
-      <c r="Y39">
-        <v>4029.2400000000002</v>
-      </c>
-      <c r="Z39">
-        <v>3861.2400000000002</v>
-      </c>
-      <c r="AA39">
-        <v>3722.3199999999997</v>
-      </c>
-      <c r="AB39">
-        <v>3673.4199999999996</v>
-      </c>
-      <c r="AC39">
-        <v>3713.5199999999995</v>
-      </c>
-      <c r="AD39">
-        <v>3700.9</v>
-      </c>
-      <c r="AE39">
-        <v>3675.6400000000003</v>
-      </c>
-      <c r="AF39">
-        <v>3673.1400000000003</v>
-      </c>
-      <c r="AG39">
-        <v>3736.0749999999998</v>
-      </c>
-      <c r="AH39">
-        <v>4539.2</v>
-      </c>
-      <c r="AI39" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ39" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK39" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL39" t="s">
-        <v>3</v>
-      </c>
-      <c r="AM39" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>56</v>
-      </c>
-      <c r="B40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40">
-        <v>196890</v>
-      </c>
-      <c r="E40">
-        <v>154441.42857142858</v>
-      </c>
-      <c r="F40">
-        <v>115399.42857142857</v>
-      </c>
-      <c r="G40">
-        <v>92991.857142857145</v>
-      </c>
-      <c r="H40">
-        <v>74232.71428571429</v>
-      </c>
-      <c r="I40">
-        <v>53431.571428571428</v>
-      </c>
-      <c r="J40">
-        <v>42975.428571428572</v>
-      </c>
-      <c r="K40">
-        <v>36493</v>
-      </c>
-      <c r="L40">
-        <v>31530.428571428572</v>
-      </c>
-      <c r="M40">
-        <v>26109.285714285714</v>
-      </c>
-      <c r="N40">
-        <v>23872</v>
-      </c>
-      <c r="O40">
-        <v>22338.857142857141</v>
-      </c>
-      <c r="P40">
-        <v>20961.857142857141</v>
-      </c>
-      <c r="Q40">
-        <v>12521.857142857143</v>
-      </c>
-      <c r="R40">
-        <v>8848.6857142857152</v>
-      </c>
-      <c r="S40" t="s">
-        <v>3</v>
-      </c>
-      <c r="T40">
-        <v>7178.6500000000005</v>
-      </c>
-      <c r="U40">
-        <v>6650.95</v>
-      </c>
-      <c r="V40">
-        <v>6408.5166666666664</v>
-      </c>
-      <c r="W40">
-        <v>6232.0999999999995</v>
-      </c>
-      <c r="X40">
-        <v>5959.3166666666666</v>
-      </c>
-      <c r="Y40">
-        <v>5609.0333333333328</v>
-      </c>
-      <c r="Z40">
-        <v>5347.6500000000005</v>
-      </c>
-      <c r="AA40">
-        <v>5139.2333333333336</v>
-      </c>
-      <c r="AB40">
-        <v>4989.0666666666666</v>
-      </c>
-      <c r="AC40">
-        <v>4886.45</v>
-      </c>
-      <c r="AD40">
-        <v>4806.5666666666666</v>
-      </c>
-      <c r="AE40">
-        <v>4726.1166666666668</v>
-      </c>
-      <c r="AF40">
-        <v>4720.8833333333332</v>
-      </c>
-      <c r="AG40">
-        <v>4716.7166666666662</v>
-      </c>
-      <c r="AH40">
-        <v>4846.25</v>
-      </c>
-      <c r="AI40">
-        <v>5233.88</v>
-      </c>
-      <c r="AJ40">
-        <v>4906.4250000000002</v>
-      </c>
-      <c r="AK40">
-        <v>5190.6499999999996</v>
-      </c>
-      <c r="AL40" t="s">
-        <v>3</v>
-      </c>
-      <c r="AM40" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41">
-        <v>196890</v>
-      </c>
-      <c r="E41">
-        <v>140595.28571428571</v>
-      </c>
-      <c r="F41">
-        <v>105145.57142857143</v>
-      </c>
-      <c r="G41">
-        <v>83181.857142857145</v>
-      </c>
-      <c r="H41">
-        <v>65106</v>
-      </c>
-      <c r="I41">
-        <v>46900.142857142855</v>
-      </c>
-      <c r="J41">
-        <v>35696.428571428572</v>
-      </c>
-      <c r="K41">
-        <v>28034.142857142859</v>
-      </c>
-      <c r="L41">
-        <v>24346</v>
-      </c>
-      <c r="M41">
-        <v>21231.857142857141</v>
-      </c>
-      <c r="N41">
-        <v>19248.714285714286</v>
-      </c>
-      <c r="O41">
-        <v>17452.714285714286</v>
-      </c>
-      <c r="P41">
-        <v>15863</v>
-      </c>
-      <c r="Q41">
-        <v>10101.785714285714</v>
-      </c>
-      <c r="R41">
-        <v>7580.5999999999995</v>
-      </c>
-      <c r="S41">
-        <v>5911.05</v>
-      </c>
-      <c r="T41">
-        <v>5293.9666666666662</v>
-      </c>
-      <c r="U41">
-        <v>4868</v>
-      </c>
-      <c r="V41">
-        <v>4575.1333333333332</v>
-      </c>
-      <c r="W41">
-        <v>4366.833333333333</v>
-      </c>
-      <c r="X41">
-        <v>4232.0166666666664</v>
-      </c>
-      <c r="Y41">
-        <v>4228.88</v>
-      </c>
-      <c r="Z41">
-        <v>4068.72</v>
-      </c>
-      <c r="AA41">
-        <v>3917.3599999999997</v>
-      </c>
-      <c r="AB41">
-        <v>3871.2599999999998</v>
-      </c>
-      <c r="AC41">
-        <v>3847.34</v>
-      </c>
-      <c r="AD41">
-        <v>3777.7599999999998</v>
-      </c>
-      <c r="AE41">
-        <v>3727.66</v>
-      </c>
-      <c r="AF41">
-        <v>3767.2249999999999</v>
-      </c>
-      <c r="AG41">
-        <v>3722.8</v>
-      </c>
-      <c r="AH41">
-        <v>3983.1333333333332</v>
-      </c>
-      <c r="AI41">
-        <v>3227.2</v>
-      </c>
-      <c r="AJ41" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK41" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL41" t="s">
-        <v>3</v>
-      </c>
-      <c r="AM41" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42">
-        <v>196890</v>
-      </c>
-      <c r="E42">
-        <v>162414.28571428571</v>
-      </c>
-      <c r="F42">
-        <v>121619.28571428571</v>
-      </c>
-      <c r="G42">
-        <v>98423.571428571435</v>
-      </c>
-      <c r="H42">
-        <v>80004.428571428565</v>
-      </c>
-      <c r="I42">
-        <v>57712.142857142855</v>
-      </c>
-      <c r="J42">
-        <v>45420.285714285717</v>
-      </c>
-      <c r="K42">
-        <v>38380.428571428572</v>
-      </c>
-      <c r="L42">
-        <v>34223.285714285717</v>
-      </c>
-      <c r="M42">
-        <v>29027.428571428572</v>
-      </c>
-      <c r="N42">
-        <v>24144.285714285714</v>
-      </c>
-      <c r="O42">
-        <v>21165.142857142859</v>
-      </c>
-      <c r="P42">
-        <v>19698.571428571428</v>
-      </c>
-      <c r="Q42">
-        <v>11703.014285714287</v>
-      </c>
-      <c r="R42">
-        <v>9118.1142857142859</v>
-      </c>
-      <c r="S42">
-        <v>7030.2285714285708</v>
-      </c>
-      <c r="T42">
-        <v>5785.5333333333328</v>
-      </c>
-      <c r="U42">
-        <v>5103.25</v>
-      </c>
-      <c r="V42">
-        <v>4779.8666666666668</v>
-      </c>
-      <c r="W42">
-        <v>4476.7666666666664</v>
-      </c>
-      <c r="X42">
-        <v>4208.1166666666668</v>
-      </c>
-      <c r="Y42">
-        <v>3887.75</v>
-      </c>
-      <c r="Z42">
-        <v>3763.4800000000005</v>
-      </c>
-      <c r="AA42">
-        <v>3538.8</v>
-      </c>
-      <c r="AB42">
-        <v>3435.95</v>
-      </c>
-      <c r="AC42">
-        <v>3368.3</v>
-      </c>
-      <c r="AD42">
-        <v>3335.5</v>
-      </c>
-      <c r="AE42">
-        <v>3175.5250000000001</v>
-      </c>
-      <c r="AF42">
-        <v>3069.5749999999998</v>
-      </c>
-      <c r="AG42">
-        <v>3358.98</v>
-      </c>
-      <c r="AH42" t="s">
-        <v>3</v>
-      </c>
-      <c r="AI42" t="s">
-        <v>3</v>
-      </c>
-      <c r="AJ42" t="s">
-        <v>3</v>
-      </c>
-      <c r="AK42" t="s">
-        <v>3</v>
-      </c>
-      <c r="AL42" t="s">
-        <v>3</v>
-      </c>
-      <c r="AM42" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Generate the average of the left and right eye for subject 29986
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/data/Curcio_1990_JCompNeurol_HumanPhotoreceptorTopography/DENSITY8_cones_resorted_computedAverage.xlsx
+++ b/data/Curcio_1990_JCompNeurol_HumanPhotoreceptorTopography/DENSITY8_cones_resorted_computedAverage.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="58">
   <si>
     <t>ALL</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>retinalDegree</t>
+  </si>
+  <si>
+    <t>29986A</t>
   </si>
 </sst>
 </file>
@@ -512,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM38"/>
+  <dimension ref="A1:AM42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5153,6 +5156,607 @@
         <v>3</v>
       </c>
     </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39">
+        <f>AVERAGE(D3,D7)</f>
+        <v>178311</v>
+      </c>
+      <c r="E39">
+        <f t="shared" ref="E39:AM42" si="4">AVERAGE(E3,E7)</f>
+        <v>148731</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="4"/>
+        <v>113608</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="4"/>
+        <v>92163.4</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="4"/>
+        <v>73105.950000000012</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="4"/>
+        <v>51919.85</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="4"/>
+        <v>41384.85</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="4"/>
+        <v>30790.55</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="4"/>
+        <v>26750.85</v>
+      </c>
+      <c r="M39">
+        <f t="shared" si="4"/>
+        <v>23609.300000000003</v>
+      </c>
+      <c r="N39">
+        <f t="shared" si="4"/>
+        <v>20753.599999999999</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="4"/>
+        <v>18593.349999999999</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="4"/>
+        <v>17041.099999999999</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="4"/>
+        <v>9197.2200000000012</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="4"/>
+        <v>7240.34</v>
+      </c>
+      <c r="S39">
+        <f t="shared" si="4"/>
+        <v>6135.5450000000001</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="4"/>
+        <v>5524.3450000000003</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="4"/>
+        <v>4519.8149999999996</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="4"/>
+        <v>4303.57</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="4"/>
+        <v>4177.3450000000003</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="4"/>
+        <v>4082.0199999999995</v>
+      </c>
+      <c r="Y39">
+        <f t="shared" si="4"/>
+        <v>3918.9700000000003</v>
+      </c>
+      <c r="Z39">
+        <f t="shared" si="4"/>
+        <v>3682.04</v>
+      </c>
+      <c r="AA39">
+        <f t="shared" si="4"/>
+        <v>3381.27</v>
+      </c>
+      <c r="AB39">
+        <f t="shared" si="4"/>
+        <v>3073.645</v>
+      </c>
+      <c r="AC39">
+        <f t="shared" si="4"/>
+        <v>2999.915</v>
+      </c>
+      <c r="AD39">
+        <f t="shared" si="4"/>
+        <v>2912.3050000000003</v>
+      </c>
+      <c r="AE39">
+        <f t="shared" si="4"/>
+        <v>2877.4700000000003</v>
+      </c>
+      <c r="AF39">
+        <f t="shared" si="4"/>
+        <v>2819.7750000000001</v>
+      </c>
+      <c r="AG39">
+        <f t="shared" si="4"/>
+        <v>2793.99</v>
+      </c>
+      <c r="AH39">
+        <f t="shared" si="4"/>
+        <v>2765.55</v>
+      </c>
+      <c r="AI39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL39" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40">
+        <f t="shared" ref="D40:S42" si="5">AVERAGE(D4,D8)</f>
+        <v>178311</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="5"/>
+        <v>166518.5</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="5"/>
+        <v>123091.5</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="5"/>
+        <v>100429.25</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="5"/>
+        <v>81146.549999999988</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="5"/>
+        <v>52253.75</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="5"/>
+        <v>38714.300000000003</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="5"/>
+        <v>31638.75</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="5"/>
+        <v>28529.85</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="5"/>
+        <v>26792.3</v>
+      </c>
+      <c r="N40">
+        <f t="shared" si="5"/>
+        <v>24269.7</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="5"/>
+        <v>21756.35</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="5"/>
+        <v>20250.099999999999</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="5"/>
+        <v>11384.75</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="5"/>
+        <v>7553.63</v>
+      </c>
+      <c r="S40" t="s">
+        <v>3</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="4"/>
+        <v>6546.88</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="4"/>
+        <v>6543.66</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="4"/>
+        <v>6500.1550000000007</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="4"/>
+        <v>6176.7849999999999</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="4"/>
+        <v>5841.5650000000005</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" si="4"/>
+        <v>5691.875</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" si="4"/>
+        <v>5429.5649999999996</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="4"/>
+        <v>5129.9949999999999</v>
+      </c>
+      <c r="AB40">
+        <f t="shared" si="4"/>
+        <v>4860.8249999999998</v>
+      </c>
+      <c r="AC40">
+        <f t="shared" si="4"/>
+        <v>4735.74</v>
+      </c>
+      <c r="AD40">
+        <f t="shared" si="4"/>
+        <v>4775.7700000000004</v>
+      </c>
+      <c r="AE40">
+        <f t="shared" si="4"/>
+        <v>4814.4650000000001</v>
+      </c>
+      <c r="AF40">
+        <f t="shared" si="4"/>
+        <v>4785.18</v>
+      </c>
+      <c r="AG40">
+        <f t="shared" si="4"/>
+        <v>4720.5200000000004</v>
+      </c>
+      <c r="AH40">
+        <f t="shared" si="4"/>
+        <v>4601.1949999999997</v>
+      </c>
+      <c r="AI40">
+        <f t="shared" si="4"/>
+        <v>4480.2250000000004</v>
+      </c>
+      <c r="AJ40">
+        <f t="shared" si="4"/>
+        <v>4445.2250000000004</v>
+      </c>
+      <c r="AK40">
+        <f t="shared" si="4"/>
+        <v>3710.76</v>
+      </c>
+      <c r="AL40" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="5"/>
+        <v>178311</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="4"/>
+        <v>129608</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="4"/>
+        <v>96648.4</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="4"/>
+        <v>72426.649999999994</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="4"/>
+        <v>55374.5</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="4"/>
+        <v>39740.600000000006</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="4"/>
+        <v>26003.599999999999</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="4"/>
+        <v>22620.6</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="4"/>
+        <v>20444.849999999999</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="4"/>
+        <v>18704.800000000003</v>
+      </c>
+      <c r="N41">
+        <f t="shared" si="4"/>
+        <v>17298</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="4"/>
+        <v>15745.7</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="4"/>
+        <v>14949.65</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="4"/>
+        <v>9653.68</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="4"/>
+        <v>6977.23</v>
+      </c>
+      <c r="S41">
+        <f t="shared" si="4"/>
+        <v>5447.9850000000006</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="4"/>
+        <v>4519.0750000000007</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="4"/>
+        <v>4148.32</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="4"/>
+        <v>3961.105</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="4"/>
+        <v>3811.1149999999998</v>
+      </c>
+      <c r="X41">
+        <f t="shared" si="4"/>
+        <v>3669.8049999999998</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" si="4"/>
+        <v>3518.5949999999998</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" si="4"/>
+        <v>3378.415</v>
+      </c>
+      <c r="AA41">
+        <f t="shared" si="4"/>
+        <v>3254.585</v>
+      </c>
+      <c r="AB41">
+        <f t="shared" si="4"/>
+        <v>3130.76</v>
+      </c>
+      <c r="AC41">
+        <f t="shared" si="4"/>
+        <v>3070.38</v>
+      </c>
+      <c r="AD41">
+        <f t="shared" si="4"/>
+        <v>2994.895</v>
+      </c>
+      <c r="AE41">
+        <f t="shared" si="4"/>
+        <v>2916.29</v>
+      </c>
+      <c r="AF41">
+        <f t="shared" si="4"/>
+        <v>2841.37</v>
+      </c>
+      <c r="AG41">
+        <f t="shared" si="4"/>
+        <v>2817.8249999999998</v>
+      </c>
+      <c r="AH41">
+        <f t="shared" si="4"/>
+        <v>2783.24</v>
+      </c>
+      <c r="AI41">
+        <f t="shared" si="4"/>
+        <v>2745.95</v>
+      </c>
+      <c r="AJ41" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK41" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL41" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="5"/>
+        <v>178311</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="4"/>
+        <v>146816</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="4"/>
+        <v>112151.5</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="4"/>
+        <v>91568.9</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="4"/>
+        <v>76838.100000000006</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="4"/>
+        <v>57053.100000000006</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="4"/>
+        <v>42139.7</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="4"/>
+        <v>36783.699999999997</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="4"/>
+        <v>32194.75</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="4"/>
+        <v>27327.699999999997</v>
+      </c>
+      <c r="N42">
+        <f t="shared" si="4"/>
+        <v>22495.9</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="4"/>
+        <v>18874.150000000001</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="4"/>
+        <v>18185.8</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="4"/>
+        <v>10632.98</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="4"/>
+        <v>7915.5949999999993</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="4"/>
+        <v>6354.88</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="4"/>
+        <v>5304.0150000000003</v>
+      </c>
+      <c r="U42">
+        <f t="shared" si="4"/>
+        <v>4603.82</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="4"/>
+        <v>4198.29</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="4"/>
+        <v>3948.7750000000001</v>
+      </c>
+      <c r="X42">
+        <f t="shared" si="4"/>
+        <v>3819.6499999999996</v>
+      </c>
+      <c r="Y42">
+        <f t="shared" si="4"/>
+        <v>3696.7349999999997</v>
+      </c>
+      <c r="Z42">
+        <f t="shared" si="4"/>
+        <v>3337.3249999999998</v>
+      </c>
+      <c r="AA42">
+        <f t="shared" si="4"/>
+        <v>2979.74</v>
+      </c>
+      <c r="AB42">
+        <f t="shared" si="4"/>
+        <v>2785.51</v>
+      </c>
+      <c r="AC42">
+        <f t="shared" si="4"/>
+        <v>2528.9450000000002</v>
+      </c>
+      <c r="AD42">
+        <f t="shared" si="4"/>
+        <v>2434.8950000000004</v>
+      </c>
+      <c r="AE42">
+        <f t="shared" si="4"/>
+        <v>2397.4549999999999</v>
+      </c>
+      <c r="AF42">
+        <f t="shared" si="4"/>
+        <v>2549.2150000000001</v>
+      </c>
+      <c r="AG42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL42" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM42" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Remade the data files with mm support (instead of retinal degrees)
Signed-off-by: gkaguirre <gkaguirre@me.com>
</commit_message>
<xml_diff>
--- a/data/Curcio_1990_JCompNeurol_HumanPhotoreceptorTopography/DENSITY8_cones_resorted_computedAverage.xlsx
+++ b/data/Curcio_1990_JCompNeurol_HumanPhotoreceptorTopography/DENSITY8_cones_resorted_computedAverage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="440" windowWidth="27780" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="1020" yWindow="460" windowWidth="27780" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DENSITY8_cones_resorted" sheetId="1" r:id="rId1"/>
@@ -197,10 +197,10 @@
     <t>computedAverage</t>
   </si>
   <si>
-    <t>retinalDegree</t>
+    <t>29986A</t>
   </si>
   <si>
-    <t>29986A</t>
+    <t>mm</t>
   </si>
 </sst>
 </file>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,115 +650,115 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.25</v>
+        <v>4.9750000000000003E-2</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>9.9500000000000005E-2</v>
       </c>
       <c r="G2">
-        <v>0.75</v>
+        <v>0.14924999999999999</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0.19900000000000001</v>
       </c>
       <c r="I2">
-        <v>1.5</v>
+        <v>0.29849999999999999</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>0.39800000000000002</v>
       </c>
       <c r="K2">
-        <v>2.5</v>
+        <v>0.49750000000000005</v>
       </c>
       <c r="L2">
-        <v>3</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="M2">
-        <v>3.5</v>
+        <v>0.69650000000000001</v>
       </c>
       <c r="N2">
-        <v>4</v>
+        <v>0.79600000000000004</v>
       </c>
       <c r="O2">
-        <v>4.5</v>
+        <v>0.89550000000000007</v>
       </c>
       <c r="P2">
-        <v>5</v>
+        <v>0.99500000000000011</v>
       </c>
       <c r="Q2">
-        <v>10</v>
+        <v>1.9900000000000002</v>
       </c>
       <c r="R2">
-        <v>15</v>
+        <v>2.9850000000000003</v>
       </c>
       <c r="S2">
-        <v>20</v>
+        <v>3.9800000000000004</v>
       </c>
       <c r="T2">
-        <v>25</v>
+        <v>4.9750000000000005</v>
       </c>
       <c r="U2">
-        <v>30</v>
+        <v>5.9700000000000006</v>
       </c>
       <c r="V2">
-        <v>35</v>
+        <v>6.9650000000000007</v>
       </c>
       <c r="W2">
-        <v>40</v>
+        <v>7.9600000000000009</v>
       </c>
       <c r="X2">
-        <v>45</v>
+        <v>8.9550000000000001</v>
       </c>
       <c r="Y2">
-        <v>50</v>
+        <v>9.9500000000000011</v>
       </c>
       <c r="Z2">
-        <v>55</v>
+        <v>10.945</v>
       </c>
       <c r="AA2">
-        <v>60</v>
+        <v>11.940000000000001</v>
       </c>
       <c r="AB2">
-        <v>65</v>
+        <v>12.935</v>
       </c>
       <c r="AC2">
-        <v>70</v>
+        <v>13.930000000000001</v>
       </c>
       <c r="AD2">
-        <v>75</v>
+        <v>14.925000000000001</v>
       </c>
       <c r="AE2">
-        <v>80</v>
+        <v>15.920000000000002</v>
       </c>
       <c r="AF2">
-        <v>85</v>
+        <v>16.914999999999999</v>
       </c>
       <c r="AG2">
-        <v>90</v>
+        <v>17.91</v>
       </c>
       <c r="AH2">
-        <v>95</v>
+        <v>18.905000000000001</v>
       </c>
       <c r="AI2">
-        <v>100</v>
+        <v>19.900000000000002</v>
       </c>
       <c r="AJ2">
-        <v>105</v>
+        <v>20.895</v>
       </c>
       <c r="AK2">
-        <v>110</v>
+        <v>21.89</v>
       </c>
       <c r="AL2">
-        <v>115</v>
+        <v>22.885000000000002</v>
       </c>
       <c r="AM2">
-        <v>120</v>
+        <v>23.880000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.2">
@@ -5158,7 +5158,7 @@
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
         <v>2</v>
@@ -5171,7 +5171,7 @@
         <v>178311</v>
       </c>
       <c r="E39">
-        <f t="shared" ref="E39:AM42" si="4">AVERAGE(E3,E7)</f>
+        <f t="shared" ref="E39:AK42" si="4">AVERAGE(E3,E7)</f>
         <v>148731</v>
       </c>
       <c r="F39">
@@ -5308,7 +5308,7 @@
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
         <v>4</v>
@@ -5317,7 +5317,7 @@
         <v>14</v>
       </c>
       <c r="D40">
-        <f t="shared" ref="D40:S42" si="5">AVERAGE(D4,D8)</f>
+        <f t="shared" ref="D40:R42" si="5">AVERAGE(D4,D8)</f>
         <v>178311</v>
       </c>
       <c r="E40">
@@ -5460,7 +5460,7 @@
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
@@ -5611,7 +5611,7 @@
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>

</xml_diff>